<commit_message>
delete overlap goal algorithm - use planning loop instread of handle_with_exceptions - add additional goal constraint satisfy condition - change cloudMap_v08.xlsx
</commit_message>
<xml_diff>
--- a/cloudMap_v08.xlsx
+++ b/cloudMap_v08.xlsx
@@ -179,7 +179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -212,10 +212,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,10 +241,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,12 +262,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -341,19 +333,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.609375" defaultRowHeight="17.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="17.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,7 +498,7 @@
       <c r="E4" s="4" t="n">
         <v>233</v>
       </c>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="4" t="n">
         <v>234</v>
       </c>
       <c r="G4" s="4" t="n">
@@ -624,43 +618,43 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="9" t="s">
+      <c r="B7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -668,34 +662,34 @@
       <c r="A8" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12" t="n">
+      <c r="B8" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="n">
         <v>206</v>
       </c>
-      <c r="F8" s="12" t="n">
+      <c r="F8" s="11" t="n">
         <v>207</v>
       </c>
-      <c r="G8" s="12" t="n">
+      <c r="G8" s="11" t="n">
         <v>208</v>
       </c>
-      <c r="H8" s="12" t="n">
+      <c r="H8" s="11" t="n">
         <v>209</v>
       </c>
-      <c r="I8" s="12" t="n">
+      <c r="I8" s="11" t="n">
         <v>210</v>
       </c>
-      <c r="J8" s="12" t="n">
+      <c r="J8" s="11" t="n">
         <v>211</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K8" s="12" t="n">
         <v>212</v>
       </c>
       <c r="L8" s="1" t="s">
@@ -712,37 +706,37 @@
       <c r="A9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12" t="n">
+      <c r="B9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11" t="n">
         <v>205</v>
       </c>
-      <c r="E9" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="14" t="n">
+      <c r="E9" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="14" t="n">
+      <c r="G9" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="14" t="n">
+      <c r="H9" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="I9" s="14" t="n">
+      <c r="I9" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="J9" s="14" t="n">
+      <c r="J9" s="13" t="n">
         <v>6</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="13" t="n">
+      <c r="L9" s="12" t="n">
         <v>214</v>
       </c>
       <c r="M9" s="1" t="s">
@@ -756,28 +750,28 @@
       <c r="A10" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B10" s="15" t="n">
+      <c r="B10" s="14" t="n">
         <v>101</v>
       </c>
-      <c r="C10" s="13" t="n">
+      <c r="C10" s="12" t="n">
         <v>201</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="12" t="n">
         <v>213</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="14" t="n">
+      <c r="F10" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="G10" s="14" t="n">
+      <c r="G10" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="H10" s="14" t="n">
+      <c r="H10" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="I10" s="14" t="n">
+      <c r="I10" s="13" t="n">
         <v>10</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -786,13 +780,13 @@
       <c r="K10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L10" s="13" t="n">
+      <c r="L10" s="12" t="n">
         <v>223</v>
       </c>
-      <c r="M10" s="13" t="n">
+      <c r="M10" s="12" t="n">
         <v>225</v>
       </c>
-      <c r="N10" s="14" t="n">
+      <c r="N10" s="13" t="n">
         <v>18</v>
       </c>
     </row>
@@ -800,88 +794,88 @@
       <c r="A11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="12" t="n">
         <v>215</v>
       </c>
-      <c r="E11" s="17" t="n">
+      <c r="E11" s="12" t="n">
         <v>216</v>
       </c>
-      <c r="F11" s="13" t="n">
+      <c r="F11" s="12" t="n">
         <v>217</v>
       </c>
-      <c r="G11" s="13" t="n">
+      <c r="G11" s="12" t="n">
         <v>218</v>
       </c>
-      <c r="H11" s="13" t="n">
+      <c r="H11" s="12" t="n">
         <v>219</v>
       </c>
-      <c r="I11" s="13" t="n">
+      <c r="I11" s="12" t="n">
         <v>220</v>
       </c>
-      <c r="J11" s="13" t="n">
+      <c r="J11" s="12" t="n">
         <v>221</v>
       </c>
-      <c r="K11" s="13" t="n">
+      <c r="K11" s="12" t="n">
         <v>222</v>
       </c>
-      <c r="L11" s="13" t="n">
-        <v>224</v>
-      </c>
-      <c r="M11" s="13" t="n">
-        <v>226</v>
-      </c>
-      <c r="N11" s="14" t="n">
-        <v>19</v>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B12" s="18" t="n">
+      <c r="B12" s="16" t="n">
         <v>102</v>
       </c>
-      <c r="C12" s="19" t="n">
+      <c r="C12" s="17" t="n">
         <v>202</v>
       </c>
-      <c r="D12" s="19" t="n">
+      <c r="D12" s="17" t="n">
         <v>227</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>228</v>
       </c>
-      <c r="F12" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="14" t="n">
+      <c r="F12" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13" t="n">
         <v>11</v>
       </c>
-      <c r="H12" s="14" t="n">
+      <c r="H12" s="13" t="n">
         <v>12</v>
       </c>
-      <c r="I12" s="14" t="n">
+      <c r="I12" s="13" t="n">
         <v>13</v>
       </c>
-      <c r="J12" s="14" t="n">
+      <c r="J12" s="13" t="n">
         <v>14</v>
       </c>
-      <c r="K12" s="14" t="n">
+      <c r="K12" s="13" t="n">
         <v>15</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>1</v>
+      <c r="L12" s="12" t="n">
+        <v>224</v>
+      </c>
+      <c r="M12" s="12" t="n">
+        <v>226</v>
+      </c>
+      <c r="N12" s="13" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -897,7 +891,7 @@
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="21" t="n">
+      <c r="E13" s="19" t="n">
         <v>22</v>
       </c>
       <c r="F13" s="1" t="s">

</xml_diff>